<commit_message>
Fixed jar output and added basic filename reading input from command-line arguments.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>Team 1</t>
   </si>
@@ -35,109 +35,115 @@
     <t>102-BULLS-SHORTER</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>8:00</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=28,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>103-EAGLES-CROWE</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=9,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>104-GAUCHOS</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=5,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>105-IRISH-WEBSTER 1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=8,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>106-PATRIOTS</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=16,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>107-SHOOTIN TIGERS-JENNINGS</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=0,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=2,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>Oct.4</t>
-  </si>
-  <si>
-    <t>103-EAGLES-CROWE</t>
-  </si>
-  <si>
-    <t>20:00</t>
-  </si>
-  <si>
-    <t>Oct.14</t>
-  </si>
-  <si>
-    <t>104-GAUCHOS</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>21:00</t>
-  </si>
-  <si>
-    <t>Oct.19</t>
-  </si>
-  <si>
-    <t>105-IRISH-WEBSTER 1</t>
-  </si>
-  <si>
-    <t>6:00</t>
-  </si>
-  <si>
-    <t>Oct.2</t>
-  </si>
-  <si>
-    <t>106-PATRIOTS</t>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=15,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=20,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
   </si>
   <si>
     <t>23:00</t>
   </si>
   <si>
-    <t>Oct.12</t>
-  </si>
-  <si>
-    <t>107-SHOOTIN TIGERS-JENNINGS</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>Oct.20</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=3,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=29,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>0:00</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=12,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>22:00</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=25,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=14,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
+  </si>
+  <si>
+    <t>java.util.GregorianCalendar[time=?,areFieldsSet=false,areAllFieldsSet=true,lenient=true,zone=sun.util.calendar.ZoneInfo[id="America/Chicago",offset=-21600000,dstSavings=3600000,useDaylight=true,transitions=235,lastRule=java.util.SimpleTimeZone[id=America/Chicago,offset=-21600000,dstSavings=3600000,useDaylight=true,startYear=0,startMode=3,startMonth=2,startDay=8,startDayOfWeek=1,startTime=7200000,startTimeMode=0,endMode=3,endMonth=10,endDay=1,endDayOfWeek=1,endTime=7200000,endTimeMode=0]],firstDayOfWeek=1,minimalDaysInFirstWeek=1,ERA=1,YEAR=2013,MONTH=9,WEEK_OF_YEAR=42,WEEK_OF_MONTH=3,DAY_OF_MONTH=27,DAY_OF_YEAR=289,DAY_OF_WEEK=4,DAY_OF_WEEK_IN_MONTH=3,AM_PM=0,HOUR=10,HOUR_OF_DAY=10,MINUTE=36,SECOND=8,MILLISECOND=589,ZONE_OFFSET=-21600000,DST_OFFSET=3600000]</t>
   </si>
   <si>
     <t>4:00</t>
   </si>
   <si>
-    <t>Oct.17</t>
-  </si>
-  <si>
-    <t>Oct.27</t>
-  </si>
-  <si>
-    <t>22:00</t>
-  </si>
-  <si>
-    <t>Oct.6</t>
-  </si>
-  <si>
-    <t>7:00</t>
-  </si>
-  <si>
-    <t>Oct.30</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>12:00</t>
-  </si>
-  <si>
-    <t>Oct.23</t>
-  </si>
-  <si>
-    <t>16:00</t>
-  </si>
-  <si>
-    <t>Oct.5</t>
-  </si>
-  <si>
-    <t>Oct.18</t>
-  </si>
-  <si>
-    <t>8:00</t>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>2:00</t>
   </si>
 </sst>
 </file>
@@ -230,13 +236,13 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -244,16 +250,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -261,16 +267,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
@@ -278,16 +284,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -295,16 +301,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
@@ -315,13 +321,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
@@ -329,13 +335,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -346,16 +352,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -363,16 +369,16 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -380,16 +386,16 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -397,16 +403,16 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
         <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -414,16 +420,16 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
@@ -431,16 +437,16 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16">
@@ -448,118 +454,118 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
         <v>38</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1129967 #1158450 #420 #YOLO #SWAG  The solver engine now tries to solve when run (though scores aren't calculated correctly still). Paired with Matthew Swinney.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
   <si>
     <t>Team 1</t>
   </si>
@@ -27,6 +27,27 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>101-BLACK AND WHITE TIGERS</t>
+  </si>
+  <si>
+    <t>102-BULLS-SHORTER</t>
+  </si>
+  <si>
+    <t>103-EAGLES-CROWE</t>
+  </si>
+  <si>
+    <t>104-GAUCHOS</t>
+  </si>
+  <si>
+    <t>105-IRISH-WEBSTER 1</t>
+  </si>
+  <si>
+    <t>106-PATRIOTS</t>
+  </si>
+  <si>
+    <t>107-SHOOTIN TIGERS-JENNINGS</t>
   </si>
 </sst>
 </file>
@@ -94,6 +115,363 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>